<commit_message>
updates to README and ambiguity check feature
</commit_message>
<xml_diff>
--- a/data/combined_output.xlsx
+++ b/data/combined_output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_traceability_project/traceability_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD3F0DB0E7BFB381159BBA8777A61E260" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{275DFAF4-0DC6-416E-A59A-950BED6C3993}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_3F9DB3A8D3105B228F1B3C11595ED87656CD301C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4523F5C5-4422-4C06-989E-550A25BF043B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>requirements</t>
   </si>
@@ -28,46 +28,148 @@
     <t>Section_2_4.txt</t>
   </si>
   <si>
+    <t>Section_4_3_1.txt</t>
+  </si>
+  <si>
+    <t>Section_4_3_2.txt</t>
+  </si>
+  <si>
+    <t>Section_4_3_3.txt</t>
+  </si>
+  <si>
+    <t>Section_4_3_4.txt</t>
+  </si>
+  <si>
+    <t>Section_4_3_5.txt</t>
+  </si>
+  <si>
+    <t>Section_4_3_6.txt</t>
+  </si>
+  <si>
     <t>reviews</t>
   </si>
   <si>
     <t>revision</t>
   </si>
   <si>
-    <t>Program Administrators and Nursing Staff Members shall be able to specify the preferred sequence of classes for a given cohort.</t>
-  </si>
-  <si>
-    <t>The requirement includes the roles "Program Administrators" and "Nursing Staff Members", but does not specify what "preferred sequence of classes" means. It lacks clarity on how this preference is established or prioritized, leading to possible multiple interpretations of what these roles can specify. Recommendations include defining what constitutes a "preferred sequence" and how it will be determined to remove ambiguity.</t>
-  </si>
-  <si>
-    <t>Program Administrators and Nursing Staff Members shall be able to specify the preferred sequence of classes for a given cohort, where the "preferred sequence" is defined as a prioritized list of classes established based on predefined criteria such as availability, prerequisites, and user input.</t>
-  </si>
-  <si>
-    <t>The product shall allow a user to identify himself or herself as a player.</t>
-  </si>
-  <si>
-    <t>The phrase "identify himself or herself" is ambiguous as it does not clarify the method of identification. This could include username, email, or another identifier. Consider rephrasing to specify the identification method (e.g., "the product shall allow a user to enter a username or email to identify as a player") to enhance clarity and reduce ambiguity.</t>
-  </si>
-  <si>
-    <t>The product shall allow a user to enter a username or email to identify as a player.</t>
-  </si>
-  <si>
     <t>The Disputes System shall provide view access capability for authorized users of the application.</t>
   </si>
   <si>
-    <t>The term "view access capability" is not well-defined. It is unclear what constitutes "view access" (e.g., permissions for viewing documents, records, etc.). Recommend detailing what specific content is accessible and what "authorized users" entail to ensure a singular interpretation.</t>
-  </si>
-  <si>
-    <t>The Disputes System shall provide view access capability for authorized users of the application, where "view access" is defined as the ability to view specific content types such as documents and records, as determined by user permissions.</t>
-  </si>
-  <si>
-    <t>The ratings shall include categories for attempted use of recycled parts and actual use of recycled parts.</t>
-  </si>
-  <si>
-    <t>The terms "attempted use" and "actual use" may be interpreted differently by users. It is unclear what metrics or evidence will determine whether the use was "attempted" versus "actual". Suggestions for improvement include specifying criteria for categorization to eliminate confusion.</t>
-  </si>
-  <si>
-    <t>The ratings shall include categories for "attempted use of recycled parts" and "actual use of recycled parts," with specific criteria defined to distinguish between "attempted" and "actual use," such as documented evidence or metrics of recycling.</t>
+    <t>The requirement is somewhat ambiguous regarding what constitutes "view access capability." It should specify the types of data or sections of the application that authorized users can view to eliminate any assumptions about the extent of access.</t>
+  </si>
+  <si>
+    <t>The grammar is correct; however, the term "access capability" may cause ambiguity. It would improve clarity to specify what "view access" entails, such as which data can be viewed or any constraints that might apply.</t>
+  </si>
+  <si>
+    <t>The requirement is acceptable in spelling and capitalization; however, it could be improved by specifying what 'view access capability' entails. Defining 'authorized users' and providing clarity on what access details fall under 'view' would further enhance verifiability.</t>
+  </si>
+  <si>
+    <t>The requirement is punctuated correctly, providing clarity. However, the phrase "view access capability" could be more specific by defining what "view access" entails. A glossary reference for "authorized users" should also be included to ensure clarity.</t>
+  </si>
+  <si>
+    <t>The requirement is clear but does not utilize any logical expression; since it is a singular thought, it does not require improvement. No ambiguity is present.</t>
+  </si>
+  <si>
+    <t>The requirement does not use the word not, so it is clear, verifiable, and aligns with the positive framing encouraged by the context. However, to enhance clarity, specify what "view access capability" entails.</t>
+  </si>
+  <si>
+    <t>The requirement is acceptable as it does not use the oblique symbol. However, it could be improved by explicitly defining what constitutes "view access capability" to prevent ambiguity.</t>
+  </si>
+  <si>
+    <t>The requirement is somewhat ambiguous regarding what constitutes "view access capability." It should specify the types of data or sections of the application that authorized users can view to eliminate any assumptions about the extent of access. The grammar is correct; however, the term "access capability" may cause ambiguity. It would improve clarity to specify what "view access" entails, such as which data can be viewed or any constraints that might apply. The requirement is acceptable in spelling and capitalization; however, it could be improved by specifying what 'view access capability' entails. Defining 'authorized users' and providing clarity on what access details fall under 'view' would further enhance verifiability. The requirement is punctuated correctly, providing clarity. However, the phrase "view access capability" could be more specific by defining what "view access" entails. A glossary reference for "authorized users" should also be included to ensure clarity. The requirement is clear but does not utilize any logical expression; since it is a singular thought, it does not require improvement. No ambiguity is present. The requirement does not use the word not, so it is clear, verifiable, and aligns with the positive framing encouraged by the context. However, to enhance clarity, specify what "view access capability" entails. The requirement is acceptable as it does not use the oblique symbol. However, it could be improved by explicitly defining what constitutes "view access capability" to prevent ambiguity.</t>
+  </si>
+  <si>
+    <t>The Disputes System shall provide view access capability for authorized users of the application, specifying the types of data or sections of the application that can be viewed and defining "authorized users" for clarity.</t>
+  </si>
+  <si>
+    <t>The Disputes System shall provide update access capability for authorized users of the application.</t>
+  </si>
+  <si>
+    <t>Similar to the previous requirement, the term "update access capability" is vague. The requirement should clearly define what types of updates users are permitted to make, e.g., updates to user profiles, dispute details, etc.</t>
+  </si>
+  <si>
+    <t>The grammar is correct; similar to the previous requirement, "update access capability" is vague. It is recommended to clarify which updates can be made and under what conditions to prevent misinterpretation.</t>
+  </si>
+  <si>
+    <t>Similar to Requirement A, this requirement is free from spelling errors. It would benefit from clarification on what 'update access capability' includes and how 'authorized users' are defined for better validation.</t>
+  </si>
+  <si>
+    <t>Similar to Requirement A, the punctuation is correct. The phrase "update access capability" lacks specificity and could benefit from clear definitions. A glossary reference for "authorized users" should also be included.</t>
+  </si>
+  <si>
+    <t>Similar to Requirement A, this requirement is clear and singular. It does not incorporate logical expressions and does not need improvement as it does not present ambiguity.</t>
+  </si>
+  <si>
+    <t>This requirement does not contain the word not and maintains a positive statement. To improve this requirement, consider defining the types of updates allowed for clarity and completeness.</t>
+  </si>
+  <si>
+    <t>Similar to the previous requirement, this one does not contain the oblique symbol. However, clarification on what "update access capability" includes would enhance precision.</t>
+  </si>
+  <si>
+    <t>Similar to the previous requirement, the term "update access capability" is vague. The requirement should clearly define what types of updates users are permitted to make, e.g., updates to user profiles, dispute details, etc. The grammar is correct; similar to the previous requirement, "update access capability" is vague. It is recommended to clarify which updates can be made and under what conditions to prevent misinterpretation. Similar to Requirement A, this requirement is free from spelling errors. It would benefit from clarification on what 'update access capability' includes and how 'authorized users' are defined for better validation. Similar to Requirement A, the punctuation is correct. The phrase "update access capability" lacks specificity and could benefit from clear definitions. A glossary reference for "authorized users" should also be included. Similar to Requirement A, this requirement is clear and singular. It does not incorporate logical expressions and does not need improvement as it does not present ambiguity. This requirement does not contain the word not and maintains a positive statement. To improve this requirement, consider defining the types of updates allowed for clarity and completeness. Similar to the previous requirement, this one does not contain the oblique symbol. However, clarification on what "update access capability" includes would enhance precision.</t>
+  </si>
+  <si>
+    <t>The Disputes System shall provide update access capability for authorized users of the application, clearly defining the types of updates permitted, such as updates to user profiles and dispute details, and detailing the authentication criteria for "authorized users."</t>
+  </si>
+  <si>
+    <t>The Disputes System must allow the users to select disputable transactions (based on the age of the transaction) from a user interface and initiate a dispute (ticket retrieval request or chargeback notification) on the selected transaction.</t>
+  </si>
+  <si>
+    <t>This requirement is complex and may be interpreted in multiple ways, particularly regarding "disputable transactions" and the mechanics of initiating a dispute. It should clarify the criteria for disputable transactions and detail the steps for initiating a dispute to avoid confusion on the necessary actions and features of the user interface.</t>
+  </si>
+  <si>
+    <t>The sentence structure is correct, but it is overly complex. Breaking it into two sentences for better readability is advisable. Additionally, defining “disputable transactions” and the exact meanings of "ticket retrieval request" and "chargeback notification" will enhance clarity.</t>
+  </si>
+  <si>
+    <t>The spelling is correct, but the phrase 'disputable transactions' could be specified better. The meaning of 'age of the transaction' should be clarified. Additionally, consider defining 'user interface' to ensure all stakeholders have a common understanding.</t>
+  </si>
+  <si>
+    <t>This requirement contains multiple clauses that could benefit from improved punctuation for clarity. The use of parentheses is appropriate, but separating clauses with punctuation could help prevent confusion. Consider revising for clearer structure. Also, a definition for "disputable transactions" should be included.</t>
+  </si>
+  <si>
+    <t>This requirement contains multiple thoughts connected by "and", which creates ambiguity. It could be improved by breaking it into two separate requirements or restructuring it to use logical expressions, for example, "The Disputes System must allow users to [select disputable transactions based on the age of the transaction] AND [initiate a dispute (ticket retrieval request or chargeback notification) on the selected transaction]".</t>
+  </si>
+  <si>
+    <t>This requirement is stated positively and allows for verification. However, the term "disputable transactions" could be better defined, and it may be beneficial to break this requirement into smaller, more manageable requirements for clarity and verifiability.</t>
+  </si>
+  <si>
+    <t>This requirement includes the oblique symbol in "ticket retrieval request or chargeback notification," leading to ambiguity about what actions users can take. It would be beneficial to split this requirement into two separate ones to clarify user actions: one for initiating a ticket retrieval request and another for chargeback notification.</t>
+  </si>
+  <si>
+    <t>This requirement is complex and may be interpreted in multiple ways, particularly regarding "disputable transactions" and the mechanics of initiating a dispute. It should clarify the criteria for disputable transactions and detail the steps for initiating a dispute to avoid confusion on the necessary actions and features of the user interface. The sentence structure is correct, but it is overly complex. Breaking it into two sentences for better readability is advisable. Additionally, defining “disputable transactions” and the exact meanings of "ticket retrieval request" and "chargeback notification" will enhance clarity. The spelling is correct, but the phrase 'disputable transactions' could be specified better. The meaning of 'age of the transaction' should be clarified. Additionally, consider defining 'user interface' to ensure all stakeholders have a common understanding. This requirement contains multiple clauses that could benefit from improved punctuation for clarity. The use of parentheses is appropriate, but separating clauses with punctuation could help prevent confusion. Consider revising for clearer structure. Also, a definition for "disputable transactions" should be included. This requirement contains multiple thoughts connected by "and", which creates ambiguity. It could be improved by breaking it into two separate requirements or restructuring it to use logical expressions, for example, "The Disputes System must allow users to [select disputable transactions based on the age of the transaction] AND [initiate a dispute (ticket retrieval request or chargeback notification) on the selected transaction]". This requirement is stated positively and allows for verification. However, the term "disputable transactions" could be better defined, and it may be beneficial to break this requirement into smaller, more manageable requirements for clarity and verifiability. This requirement includes the oblique symbol in "ticket retrieval request or chargeback notification," leading to ambiguity about what actions users can take. It would be beneficial to split this requirement into two separate ones to clarify user actions: one for initiating a ticket retrieval request and another for chargeback notification.</t>
+  </si>
+  <si>
+    <t>The Disputes System must allow users to select disputable transactions based on defined criteria, including the age of the transaction, and must detail the steps for initiating a dispute, which may involve a ticket retrieval request or a chargeback notification, ensuring these actions are distinct and clearly defined.</t>
+  </si>
+  <si>
+    <t>The Disputes System must provide the user the ability to initiate a single dispute case on multiple transactions that belong to a single merchant.</t>
+  </si>
+  <si>
+    <t>The phrase "multiple transactions that belong to a single merchant" could be misconstrued. Clarifying whether it refers to transactions grouped specifically by the merchant’s ID or other criteria would help eliminate ambiguity. A more precise definition would lead to clearer understanding and implementation.</t>
+  </si>
+  <si>
+    <t>The grammar is correct; however, the term "single dispute case" requires clarification. It is recommended to explicitly define what constitutes a single dispute and how it relates to multiple transactions to avoid ambiguity.</t>
+  </si>
+  <si>
+    <t>The spelling and capitalization are correct. However, the term 'single merchant' should be defined to clarify what conditions qualify a merchant as 'single'. Furthermore, additional context on how the 'dispute case' operates can improve understanding.</t>
+  </si>
+  <si>
+    <t>While the punctuation is generally correct, the phrase "the user the ability to initiate" could be more clearly stated as "the ability for the user to initiate." Additionally, consideration should be given to defining "dispute case" and "single merchant" to avoid ambiguity.</t>
+  </si>
+  <si>
+    <t>This requirement is singular and effectively communicates a clear need without the use of logical expressions. It does not require changes as it does not introduce ambiguity.</t>
+  </si>
+  <si>
+    <t>This requirement is stated positively and avoids the use of not. Consider elaborating on what constitutes a "dispute case" and the limitations, if any, on the number of transactions to ensure clarity and verifiability.</t>
+  </si>
+  <si>
+    <t>The requirement is clear and does not include the oblique symbol. However, it could be made more precise by defining what "multiple transactions" entails.</t>
+  </si>
+  <si>
+    <t>The phrase "multiple transactions that belong to a single merchant" could be misconstrued. Clarifying whether it refers to transactions grouped specifically by the merchant’s ID or other criteria would help eliminate ambiguity. A more precise definition would lead to clearer understanding and implementation. The grammar is correct; however, the term "single dispute case" requires clarification. It is recommended to explicitly define what constitutes a single dispute and how it relates to multiple transactions to avoid ambiguity. The spelling and capitalization are correct. However, the term 'single merchant' should be defined to clarify what conditions qualify a merchant as 'single'. Furthermore, additional context on how the 'dispute case' operates can improve understanding. While the punctuation is generally correct, the phrase "the user the ability to initiate" could be more clearly stated as "the ability for the user to initiate." Additionally, consideration should be given to defining "dispute case" and "single merchant" to avoid ambiguity. This requirement is singular and effectively communicates a clear need without the use of logical expressions. It does not require changes as it does not introduce ambiguity. This requirement is stated positively and avoids the use of not. Consider elaborating on what constitutes a "dispute case" and the limitations, if any, on the number of transactions to ensure clarity and verifiability. The requirement is clear and does not include the oblique symbol. However, it could be made more precise by defining what "multiple transactions" entails.</t>
+  </si>
+  <si>
+    <t>The Disputes System must provide the ability for the user to initiate a dispute case that encompasses multiple transactions associated with a specific merchant, clearly defining what constitutes a "single merchant" and what is meant by a "dispute case," including any limits on the number of transactions.</t>
   </si>
 </sst>
 </file>
@@ -123,19 +225,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,101 +535,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="52.81640625" customWidth="1"/>
-    <col min="4" max="4" width="48.7265625" customWidth="1"/>
-    <col min="5" max="5" width="79.90625" customWidth="1"/>
+    <col min="2" max="2" width="54.7265625" customWidth="1"/>
+    <col min="3" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="99.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+    <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+    <row r="3" spans="1:11" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+    <row r="4" spans="1:11" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+    <row r="5" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>